<commit_message>
order placement, fillo related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/files/ConfigSheet.xlsx
+++ b/src/test/resources/files/ConfigSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>login</t>
   </si>
@@ -138,44 +138,25 @@
     <t>https://test.redington.market/api/v1/marketPlace/keywordSearch?q=Office%20365%20Enterprise%20E3&amp;countryCode=ARE</t>
   </si>
   <si>
-    <t>burhani1060</t>
-  </si>
-  <si>
-    <t>tno400002283</t>
-  </si>
-  <si>
-    <t>vat390002403</t>
-  </si>
-  <si>
-    <t>customer1852</t>
-  </si>
-  <si>
-    <t>CompanyName119</t>
-  </si>
-  <si>
-    <t>burhani1061</t>
-  </si>
-  <si>
-    <t>tno400002284</t>
-  </si>
-  <si>
-    <t>vat390002404</t>
-  </si>
-  <si>
-    <t>customer1853</t>
-  </si>
-  <si>
-    <t>customer1854</t>
-  </si>
-  <si>
-    <t>CompanyName120</t>
+    <t>customer3061</t>
+  </si>
+  <si>
+    <t>CompanyName3029</t>
+  </si>
+  <si>
+    <t>burhani1095</t>
+  </si>
+  <si>
+    <t>tno400002318</t>
+  </si>
+  <si>
+    <t>vat390002438</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -564,15 +545,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="112.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="112.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,7 +715,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -745,7 +726,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -756,7 +737,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -789,7 +770,7 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
@@ -800,7 +781,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
credit request customer create 14/12/2017
</commit_message>
<xml_diff>
--- a/src/test/resources/files/ConfigSheet.xlsx
+++ b/src/test/resources/files/ConfigSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>login</t>
   </si>
@@ -138,25 +138,80 @@
     <t>https://test.redington.market/api/v1/marketPlace/keywordSearch?q=Office%20365%20Enterprise%20E3&amp;countryCode=ARE</t>
   </si>
   <si>
-    <t>customer3061</t>
-  </si>
-  <si>
-    <t>CompanyName3029</t>
-  </si>
-  <si>
-    <t>burhani1095</t>
-  </si>
-  <si>
-    <t>tno400002318</t>
-  </si>
-  <si>
-    <t>vat390002438</t>
+    <t>burhani7001</t>
+  </si>
+  <si>
+    <t>tno400002338</t>
+  </si>
+  <si>
+    <t>vat390002458</t>
+  </si>
+  <si>
+    <t>CompanyName7001</t>
+  </si>
+  <si>
+    <t>customer7004</t>
+  </si>
+  <si>
+    <t>burhani7002</t>
+  </si>
+  <si>
+    <t>tno400002339</t>
+  </si>
+  <si>
+    <t>vat390002459</t>
+  </si>
+  <si>
+    <t>customer7005</t>
+  </si>
+  <si>
+    <t>customer7006</t>
+  </si>
+  <si>
+    <t>CompanyName7002</t>
+  </si>
+  <si>
+    <t>customer7007</t>
+  </si>
+  <si>
+    <t>customer7008</t>
+  </si>
+  <si>
+    <t>customer7009</t>
+  </si>
+  <si>
+    <t>burhani7003</t>
+  </si>
+  <si>
+    <t>tno400002340</t>
+  </si>
+  <si>
+    <t>vat390002460</t>
+  </si>
+  <si>
+    <t>customer7010</t>
+  </si>
+  <si>
+    <t>customer7011</t>
+  </si>
+  <si>
+    <t>CompanyName7003</t>
+  </si>
+  <si>
+    <t>customer7012</t>
+  </si>
+  <si>
+    <t>customer7013</t>
+  </si>
+  <si>
+    <t>customer7014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -545,15 +600,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="112.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="112.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -715,7 +770,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -726,7 +781,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -737,7 +792,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -770,7 +825,7 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
@@ -781,7 +836,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
vat with coupan code 9jan2017
</commit_message>
<xml_diff>
--- a/src/test/resources/files/ConfigSheet.xlsx
+++ b/src/test/resources/files/ConfigSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="149">
   <si>
     <t>login</t>
   </si>
@@ -283,77 +283,193 @@
     <t>vendorId</t>
   </si>
   <si>
-    <t>AEBDB02D-BD91-469C-A8F3-C1C49E8FE9B9</t>
-  </si>
-  <si>
-    <t>4cbe5d1d-b367-4f92-8779-64b37f5681c6</t>
-  </si>
-  <si>
-    <t>TestThree8115</t>
-  </si>
-  <si>
-    <t>tno900008462</t>
-  </si>
-  <si>
-    <t>vat390008582</t>
-  </si>
-  <si>
-    <t>5a4b961076ea531f685db5f2</t>
-  </si>
-  <si>
-    <t>TestThreecustomer8149</t>
-  </si>
-  <si>
-    <t>TestThreeCompanyName8091</t>
-  </si>
-  <si>
-    <t>5a4b962476ea531f685db792</t>
-  </si>
-  <si>
-    <t>414051000000068</t>
-  </si>
-  <si>
-    <t>TestOneTestburni7126</t>
-  </si>
-  <si>
-    <t>tno900002452</t>
-  </si>
-  <si>
-    <t>vat390002572</t>
-  </si>
-  <si>
-    <t>5a4b9a3f76ea531f685db7bc</t>
-  </si>
-  <si>
-    <t>5a4b9b8a76ea531f685db95c</t>
-  </si>
-  <si>
-    <t>TestSixTestburni7127</t>
-  </si>
-  <si>
-    <t>tno060002453</t>
-  </si>
-  <si>
-    <t>vat060002573</t>
-  </si>
-  <si>
-    <t>TestSixTestburni7128</t>
-  </si>
-  <si>
-    <t>tno60002454</t>
-  </si>
-  <si>
-    <t>vat60002574</t>
-  </si>
-  <si>
-    <t>5a4b9c2e76ea531f685dbafc</t>
+    <t>414051000000072</t>
+  </si>
+  <si>
+    <t>E967D86A-BD42-4549-827F-187535B60B3C</t>
+  </si>
+  <si>
+    <t>2cacbb1c-cd95-4e41-ab32-5804bd8111af</t>
+  </si>
+  <si>
+    <t>bquantity</t>
+  </si>
+  <si>
+    <t>bdiscount</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>bprice</t>
+  </si>
+  <si>
+    <t>18.18</t>
+  </si>
+  <si>
+    <t>65-rg-0</t>
+  </si>
+  <si>
+    <t>planType</t>
+  </si>
+  <si>
+    <t>currencyCode</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>expiresOn</t>
+  </si>
+  <si>
+    <t>2019-01-03</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>addproduct</t>
+  </si>
+  <si>
+    <t>baseCouponCode</t>
+  </si>
+  <si>
+    <t>414051000000074</t>
+  </si>
+  <si>
+    <t>688568C6-26E9-4E2E-8760-00D21B40AAE4</t>
+  </si>
+  <si>
+    <t>9d77ba44-4708-47a7-8c0a-bc555eff53d7</t>
+  </si>
+  <si>
+    <t>dusername</t>
+  </si>
+  <si>
+    <t>dpassword</t>
+  </si>
+  <si>
+    <t>dbamusername</t>
+  </si>
+  <si>
+    <t>dbampassword</t>
+  </si>
+  <si>
+    <t>dcausername</t>
+  </si>
+  <si>
+    <t>dcapassword</t>
+  </si>
+  <si>
+    <t>pm3@mailinator.com</t>
+  </si>
+  <si>
+    <t>bam22nov@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@1234</t>
+  </si>
+  <si>
+    <t>ca22nov@gmail.com</t>
+  </si>
+  <si>
+    <t>TestOneTestburni7137</t>
+  </si>
+  <si>
+    <t>tno900002463</t>
+  </si>
+  <si>
+    <t>vat390002583</t>
+  </si>
+  <si>
+    <t>5a4e34d08dd0f370b3f2f1fd</t>
+  </si>
+  <si>
+    <t>TestThree8124</t>
+  </si>
+  <si>
+    <t>tno900008471</t>
+  </si>
+  <si>
+    <t>vat390008591</t>
+  </si>
+  <si>
+    <t>5a4e34ed8dd0f370b3f2f3a1</t>
+  </si>
+  <si>
+    <t>TestThreecustomer8158</t>
+  </si>
+  <si>
+    <t>TestThreeCompanyName8100</t>
+  </si>
+  <si>
+    <t>5a4e35008dd0f370b3f2f545</t>
+  </si>
+  <si>
+    <t>PlaceOrderWithVatTest</t>
+  </si>
+  <si>
+    <t>91FD106F-4B2C-4938-95AC-F54F74E9A239</t>
+  </si>
+  <si>
+    <t>Office 365 Enterprise E1</t>
+  </si>
+  <si>
+    <t>7.27</t>
+  </si>
+  <si>
+    <t>TestSevnTestburni7026</t>
+  </si>
+  <si>
+    <t>tno70002485</t>
+  </si>
+  <si>
+    <t>vat7002605</t>
+  </si>
+  <si>
+    <t>5a54c9bea73ae8605c22d66b</t>
+  </si>
+  <si>
+    <t>TestSevncustomer7025</t>
+  </si>
+  <si>
+    <t>TestSevnCompanyName7025</t>
+  </si>
+  <si>
+    <t>5a54c9d5a73ae8605c22d80f</t>
+  </si>
+  <si>
+    <t>RED-LsSrfCbSsF</t>
+  </si>
+  <si>
+    <t>TestVat7034</t>
+  </si>
+  <si>
+    <t>tno900008482</t>
+  </si>
+  <si>
+    <t>vat390008602</t>
+  </si>
+  <si>
+    <t>5a54cab4a73ae8605c22d815</t>
+  </si>
+  <si>
+    <t>5a54cacca73ae8605c22d9ba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -410,6 +526,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -749,17 +867,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="111.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="111.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -861,12 +979,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>49</v>
+        <v>111</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -874,120 +992,120 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2">
-        <v>991450</v>
+        <v>48</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>74</v>
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>75</v>
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -995,10 +1113,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1006,186 +1124,186 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
+        <v>19</v>
+      </c>
+      <c r="B24" s="2">
+        <v>991450</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>82</v>
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" t="s">
-        <v>79</v>
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>80</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="5">
-        <v>991450</v>
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="2">
-        <v>991450</v>
+        <v>42</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="5">
-        <v>60254</v>
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>57</v>
+        <v>15</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C39" t="s">
         <v>51</v>
@@ -1193,10 +1311,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="B40" s="5">
+        <v>991450</v>
       </c>
       <c r="C40" t="s">
         <v>51</v>
@@ -1204,10 +1322,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" t="s">
-        <v>98</v>
+        <v>17</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C41" t="s">
         <v>51</v>
@@ -1215,10 +1333,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>99</v>
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
       </c>
       <c r="C42" t="s">
         <v>51</v>
@@ -1226,10 +1344,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>100</v>
+        <v>19</v>
+      </c>
+      <c r="B43" s="2">
+        <v>991450</v>
       </c>
       <c r="C43" t="s">
         <v>51</v>
@@ -1237,10 +1355,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="B44" s="5">
+        <v>60254</v>
       </c>
       <c r="C44" t="s">
         <v>51</v>
@@ -1248,87 +1366,87 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="5">
-        <v>991450</v>
+        <v>56</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>59</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="2">
-        <v>991450</v>
+        <v>24</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="5">
-        <v>60254</v>
+        <v>25</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>57</v>
+        <v>15</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C52" t="s">
         <v>61</v>
@@ -1336,10 +1454,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="B53" s="5">
+        <v>991450</v>
       </c>
       <c r="C53" t="s">
         <v>61</v>
@@ -1347,10 +1465,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" t="s">
-        <v>90</v>
+        <v>17</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C54" t="s">
         <v>61</v>
@@ -1358,10 +1476,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>91</v>
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
       </c>
       <c r="C55" t="s">
         <v>61</v>
@@ -1369,10 +1487,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>92</v>
+        <v>19</v>
+      </c>
+      <c r="B56" s="2">
+        <v>991450</v>
       </c>
       <c r="C56" t="s">
         <v>61</v>
@@ -1380,10 +1498,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" t="s">
-        <v>93</v>
+        <v>53</v>
+      </c>
+      <c r="B57" s="5">
+        <v>60254</v>
       </c>
       <c r="C57" t="s">
         <v>61</v>
@@ -1391,10 +1509,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="C58" t="s">
         <v>61</v>
@@ -1402,10 +1520,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" t="s">
-        <v>95</v>
+        <v>56</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C59" t="s">
         <v>61</v>
@@ -1413,10 +1531,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="C60" t="s">
         <v>61</v>
@@ -1424,186 +1542,186 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" t="s">
-        <v>55</v>
+        <v>24</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="C66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>86</v>
-      </c>
-      <c r="B68" t="s">
-        <v>88</v>
+        <v>35</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>15</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
+      </c>
+      <c r="B70" t="s">
+        <v>70</v>
       </c>
       <c r="C70" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>52</v>
-      </c>
-      <c r="B71" s="5">
-        <v>991450</v>
+        <v>66</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
       </c>
       <c r="C71" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>17</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>19</v>
-      </c>
-      <c r="B74" s="2">
-        <v>991450</v>
+        <v>85</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="C74" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" s="5">
-        <v>60254</v>
+        <v>86</v>
+      </c>
+      <c r="B75" t="s">
+        <v>109</v>
       </c>
       <c r="C75" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C76" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>56</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>57</v>
+        <v>15</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C77" t="s">
         <v>39</v>
@@ -1611,10 +1729,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>58</v>
-      </c>
-      <c r="B78" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="B78" s="5">
+        <v>991450</v>
       </c>
       <c r="C78" t="s">
         <v>39</v>
@@ -1622,10 +1740,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>20</v>
-      </c>
-      <c r="B79" t="s">
-        <v>106</v>
+        <v>17</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -1633,10 +1751,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>24</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>107</v>
+        <v>18</v>
+      </c>
+      <c r="B80" t="s">
+        <v>21</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
@@ -1644,10 +1762,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>25</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>108</v>
+        <v>19</v>
+      </c>
+      <c r="B81" s="2">
+        <v>991450</v>
       </c>
       <c r="C81" t="s">
         <v>39</v>
@@ -1655,50 +1773,628 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="5">
+        <v>60254</v>
+      </c>
+      <c r="C82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>54</v>
+      </c>
+      <c r="B83" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>56</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C88" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>60</v>
       </c>
-      <c r="B82" t="s">
-        <v>109</v>
-      </c>
-      <c r="C82" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83" t="s">
-        <v>39</v>
+      <c r="B89" t="s">
+        <v>139</v>
+      </c>
+      <c r="C89" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>140</v>
+      </c>
+      <c r="C90" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" t="s">
+        <v>141</v>
+      </c>
+      <c r="C91" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>62</v>
+      </c>
+      <c r="B92" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>35</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>64</v>
+      </c>
+      <c r="B94" t="s">
+        <v>55</v>
+      </c>
+      <c r="C94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>67</v>
+      </c>
+      <c r="B95" t="s">
+        <v>70</v>
+      </c>
+      <c r="C95" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>66</v>
+      </c>
+      <c r="B96" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>68</v>
+      </c>
+      <c r="B97" t="s">
+        <v>71</v>
+      </c>
+      <c r="C97" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>69</v>
+      </c>
+      <c r="B98" t="s">
+        <v>73</v>
+      </c>
+      <c r="C98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" t="s">
+        <v>88</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" t="s">
+        <v>89</v>
+      </c>
+      <c r="C100" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>87</v>
+      </c>
+      <c r="B101" t="s">
+        <v>90</v>
+      </c>
+      <c r="C101" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>91</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>92</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C104" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C105" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>98</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C106" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>99</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C107" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>101</v>
+      </c>
+      <c r="C108" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>102</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C109" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>104</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C110" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>107</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>52</v>
+      </c>
+      <c r="B112" s="5">
+        <v>991450</v>
+      </c>
+      <c r="C112" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="2">
+        <v>991450</v>
+      </c>
+      <c r="C114" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>53</v>
+      </c>
+      <c r="B115" s="5">
+        <v>60254</v>
+      </c>
+      <c r="C115" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>54</v>
+      </c>
+      <c r="B116" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>56</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C117" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>58</v>
+      </c>
+      <c r="B118" t="s">
+        <v>59</v>
+      </c>
+      <c r="C118" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>20</v>
+      </c>
+      <c r="B119" t="s">
+        <v>144</v>
+      </c>
+      <c r="C119" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>24</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C120" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>25</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C121" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>60</v>
+      </c>
+      <c r="B122" t="s">
+        <v>147</v>
+      </c>
+      <c r="C122" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123" t="s">
+        <v>144</v>
+      </c>
+      <c r="C123" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>33</v>
+      </c>
+      <c r="B124" t="s">
+        <v>144</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>62</v>
+      </c>
+      <c r="B125" t="s">
+        <v>148</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>91</v>
+      </c>
+      <c r="B129" s="7">
+        <v>2</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>92</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>95</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>54</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>99</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>54</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>107</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{AAF729D0-AFD4-42A3-B018-7F55C1C71E36}"/>
-    <hyperlink ref="B12" r:id="rId2" xr:uid="{BFA4F590-0932-4CE5-AD18-E3CECCB20CAA}"/>
-    <hyperlink ref="B13" r:id="rId3" xr:uid="{19D86F18-2F76-4E4B-ACA7-AA53766677B8}"/>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{AAF729D0-AFD4-42A3-B018-7F55C1C71E36}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{BFA4F590-0932-4CE5-AD18-E3CECCB20CAA}"/>
+    <hyperlink ref="B20" r:id="rId3" xr:uid="{19D86F18-2F76-4E4B-ACA7-AA53766677B8}"/>
     <hyperlink ref="B2" r:id="rId4" xr:uid="{F6A0B376-92CA-419C-AFCB-3643361056DE}"/>
     <hyperlink ref="B3" r:id="rId5" xr:uid="{FBA490A6-71DD-45CE-8513-F0B7C722B08E}"/>
     <hyperlink ref="B9" r:id="rId6" xr:uid="{C87439F4-7D63-4103-884B-ECAFF96EEBA7}"/>
-    <hyperlink ref="B14" r:id="rId7" xr:uid="{D8CDE74E-54C3-4DAE-9627-DCB91013CA68}"/>
-    <hyperlink ref="B15" r:id="rId8" xr:uid="{8736EB81-DAF0-4FBA-92EB-770544196850}"/>
-    <hyperlink ref="B21" r:id="rId9" xr:uid="{FFEF6BC0-5FD2-41F0-A4C7-528B63CE056C}"/>
-    <hyperlink ref="B22" r:id="rId10" xr:uid="{ACF1DEF0-8CEB-4397-BA29-4B2C659A50C7}"/>
+    <hyperlink ref="B21" r:id="rId7" xr:uid="{D8CDE74E-54C3-4DAE-9627-DCB91013CA68}"/>
+    <hyperlink ref="B22" r:id="rId8" xr:uid="{8736EB81-DAF0-4FBA-92EB-770544196850}"/>
+    <hyperlink ref="B28" r:id="rId9" xr:uid="{FFEF6BC0-5FD2-41F0-A4C7-528B63CE056C}"/>
+    <hyperlink ref="B29" r:id="rId10" xr:uid="{ACF1DEF0-8CEB-4397-BA29-4B2C659A50C7}"/>
     <hyperlink ref="B4" r:id="rId11" xr:uid="{063E36DE-3F04-466E-8C9D-235695A156C7}"/>
     <hyperlink ref="B5" r:id="rId12" xr:uid="{D0264EE7-4675-4966-AD5C-A7ABA35058EC}"/>
     <hyperlink ref="B8" r:id="rId13" xr:uid="{21DF2B07-F49F-4966-B5E8-C33682421E6C}"/>
-    <hyperlink ref="B25" r:id="rId14" xr:uid="{469E98A4-3759-4562-BC08-3D639FBDC227}"/>
+    <hyperlink ref="B32" r:id="rId14" xr:uid="{469E98A4-3759-4562-BC08-3D639FBDC227}"/>
     <hyperlink ref="B6" r:id="rId15" xr:uid="{DE23C8D4-B412-4E6D-BA08-3BB3BB77C840}"/>
     <hyperlink ref="B7" r:id="rId16" xr:uid="{DB382E1D-DD62-4CFC-BF52-25BC452C4C13}"/>
-    <hyperlink ref="B32" r:id="rId17" xr:uid="{8B98AFC5-B34E-42D0-A50D-2FA2B645F40D}"/>
-    <hyperlink ref="B34" r:id="rId18" xr:uid="{68591E90-BCC3-4E3A-9216-D91915AACEB6}"/>
-    <hyperlink ref="B45" r:id="rId19" xr:uid="{80E526AC-E0A1-48C8-97FE-201CDB66D3B5}"/>
-    <hyperlink ref="B47" r:id="rId20" xr:uid="{DD60261B-36D1-4B6E-B9BB-7D13FA4CB6D5}"/>
-    <hyperlink ref="B61" r:id="rId21" xr:uid="{1B3CF9C3-FAB1-47E2-AC5D-2ADD7202492D}"/>
-    <hyperlink ref="B70" r:id="rId22" xr:uid="{1992B5E1-9C82-450D-A93C-650A87AE2691}"/>
-    <hyperlink ref="B72" r:id="rId23" xr:uid="{A282264A-35DC-4845-820E-BF7EDBB0C4F0}"/>
+    <hyperlink ref="B39" r:id="rId17" xr:uid="{8B98AFC5-B34E-42D0-A50D-2FA2B645F40D}"/>
+    <hyperlink ref="B41" r:id="rId18" xr:uid="{68591E90-BCC3-4E3A-9216-D91915AACEB6}"/>
+    <hyperlink ref="B52" r:id="rId19" xr:uid="{80E526AC-E0A1-48C8-97FE-201CDB66D3B5}"/>
+    <hyperlink ref="B54" r:id="rId20" xr:uid="{DD60261B-36D1-4B6E-B9BB-7D13FA4CB6D5}"/>
+    <hyperlink ref="B68" r:id="rId21" xr:uid="{1B3CF9C3-FAB1-47E2-AC5D-2ADD7202492D}"/>
+    <hyperlink ref="B77" r:id="rId22" xr:uid="{1992B5E1-9C82-450D-A93C-650A87AE2691}"/>
+    <hyperlink ref="B79" r:id="rId23" xr:uid="{A282264A-35DC-4845-820E-BF7EDBB0C4F0}"/>
+    <hyperlink ref="B93" r:id="rId24" xr:uid="{66EAC92E-C794-40D6-9744-8F273FCAA4A5}"/>
+    <hyperlink ref="B10" r:id="rId25" xr:uid="{625564A9-9702-4957-A50F-262581ACCFD2}"/>
+    <hyperlink ref="B11" r:id="rId26" xr:uid="{A68CCD6C-2150-49D8-AF6E-E3C0D9680201}"/>
+    <hyperlink ref="B12" r:id="rId27" xr:uid="{BE69C655-4AEC-4687-8E5C-E050721F2874}"/>
+    <hyperlink ref="B13" r:id="rId28" xr:uid="{4536D801-6FA7-4486-B0FE-C6F3C630E7D7}"/>
+    <hyperlink ref="B14" r:id="rId29" xr:uid="{A00CC206-B9EC-447C-88A1-6D9E5654E61D}"/>
+    <hyperlink ref="B15" r:id="rId30" xr:uid="{A840752A-5FC3-4D9B-ACC9-FA146422CA3B}"/>
+    <hyperlink ref="B16" r:id="rId31" xr:uid="{8B79697D-E06F-48BD-B459-456397DC6733}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 

</xml_diff>